<commit_message>
Unterkapitel zu Schnittstellen fertiggestellt
</commit_message>
<xml_diff>
--- a/Quellen und Vorlagen/Excell-Sheets/Tabellen.xlsx
+++ b/Quellen und Vorlagen/Excell-Sheets/Tabellen.xlsx
@@ -9,15 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="-4335" windowWidth="31065" windowHeight="27795" tabRatio="500" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="38400" yWindow="-4335" windowWidth="31065" windowHeight="27795" tabRatio="500" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Android Versionen" sheetId="1" r:id="rId1"/>
     <sheet name="WP_Versions" sheetId="4" r:id="rId2"/>
     <sheet name="Quellen_Reihenfolge" sheetId="3" r:id="rId3"/>
-    <sheet name="Zielplattformen" sheetId="5" r:id="rId4"/>
-    <sheet name="IOS Versionen" sheetId="2" r:id="rId5"/>
-    <sheet name="Unity_Produkte" sheetId="7" r:id="rId6"/>
+    <sheet name="Game Service" sheetId="9" r:id="rId4"/>
+    <sheet name="Schnittstellen" sheetId="8" r:id="rId5"/>
+    <sheet name="Zielplattformen" sheetId="5" r:id="rId6"/>
+    <sheet name="IOS Versionen" sheetId="2" r:id="rId7"/>
+    <sheet name="Unity_Produkte" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="317">
   <si>
     <t>Android Versionen</t>
   </si>
@@ -473,9 +475,6 @@
   </si>
   <si>
     <t>Sue Smith(2013)</t>
-  </si>
-  <si>
-    <t>the iphone wiki(2015</t>
   </si>
   <si>
     <t>Oracle - Java SE(2015)</t>
@@ -810,9 +809,6 @@
     <t>Gesamt</t>
   </si>
   <si>
-    <t>libGDX(2015)</t>
-  </si>
-  <si>
     <t>Personal Edition</t>
   </si>
   <si>
@@ -900,10 +896,94 @@
     <t>Brown(2015)</t>
   </si>
   <si>
-    <t>Unity3D(2015)d</t>
-  </si>
-  <si>
     <t>Skeet(2014)</t>
+  </si>
+  <si>
+    <t>Schnittstelle</t>
+  </si>
+  <si>
+    <t>libGDX</t>
+  </si>
+  <si>
+    <t>Cocos2D-X</t>
+  </si>
+  <si>
+    <t>Accelerometer</t>
+  </si>
+  <si>
+    <t>Gyroskop</t>
+  </si>
+  <si>
+    <t>Kompass</t>
+  </si>
+  <si>
+    <t>Kamera</t>
+  </si>
+  <si>
+    <t>Netzwerkverbindung</t>
+  </si>
+  <si>
+    <t>Geoposition</t>
+  </si>
+  <si>
+    <t>Bluetooth</t>
+  </si>
+  <si>
+    <t>Vibration</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Cocos2D-X(2015)d</t>
+  </si>
+  <si>
+    <t>libGDX(2013)b</t>
+  </si>
+  <si>
+    <t>libGDX(2013)a</t>
+  </si>
+  <si>
+    <t>Unity3D(2014)d</t>
+  </si>
+  <si>
+    <t>Unity3D(2015)e</t>
+  </si>
+  <si>
+    <t>the iphone wiki(2015)</t>
+  </si>
+  <si>
+    <t>Game Service</t>
+  </si>
+  <si>
+    <t>Erfolge</t>
+  </si>
+  <si>
+    <t>Bestenlisten</t>
+  </si>
+  <si>
+    <t>Multiplayer - Echtzeit</t>
+  </si>
+  <si>
+    <t>Multiplayer - Rundenbasiert</t>
+  </si>
+  <si>
+    <t>Spielstand sichern</t>
+  </si>
+  <si>
+    <t>Events</t>
+  </si>
+  <si>
+    <t>Analyse Spielerverhalten</t>
+  </si>
+  <si>
+    <t>Shop System</t>
+  </si>
+  <si>
+    <t>Freundesliste</t>
+  </si>
+  <si>
+    <t>Soziale Netzwerke</t>
   </si>
 </sst>
 </file>
@@ -1955,32 +2035,32 @@
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="31" t="s">
         <v>175</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>173</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C4" s="30">
         <v>40624</v>
@@ -1988,7 +2068,7 @@
     </row>
     <row r="5" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="32" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C5" s="30">
         <v>40666</v>
@@ -1996,7 +2076,7 @@
     </row>
     <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C6" s="33">
         <v>40787</v>
@@ -2004,10 +2084,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C7" s="30">
         <v>40813</v>
@@ -2015,7 +2095,7 @@
     </row>
     <row r="8" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="32" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C8" s="30">
         <v>40864</v>
@@ -2023,7 +2103,7 @@
     </row>
     <row r="9" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C9" s="30">
         <v>40912</v>
@@ -2031,7 +2111,7 @@
     </row>
     <row r="10" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C10" s="33">
         <v>41061</v>
@@ -2040,10 +2120,10 @@
     </row>
     <row r="11" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C11" s="30">
         <v>41087</v>
@@ -2051,7 +2131,7 @@
     </row>
     <row r="12" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C12" s="35">
         <v>41136</v>
@@ -2060,18 +2140,18 @@
     </row>
     <row r="13" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B13" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="C13" s="36" t="s">
         <v>189</v>
-      </c>
-      <c r="C13" s="36" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C14" s="30">
         <v>41304</v>
@@ -2079,7 +2159,7 @@
     </row>
     <row r="15" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C15" s="37">
         <v>41347</v>
@@ -2088,40 +2168,40 @@
     </row>
     <row r="16" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B16" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="C16" s="36" t="s">
         <v>194</v>
-      </c>
-      <c r="C16" s="36" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="39" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B17" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="C17" s="32" t="s">
         <v>196</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="B18" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="C18" s="32" t="s">
         <v>199</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="39" t="s">
+        <v>200</v>
+      </c>
+      <c r="B19" s="32" t="s">
         <v>201</v>
-      </c>
-      <c r="B19" s="32" t="s">
-        <v>202</v>
       </c>
       <c r="C19" s="40">
         <v>41474</v>
@@ -2129,34 +2209,34 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="39" t="s">
+        <v>204</v>
+      </c>
+      <c r="B21" s="32" t="s">
         <v>205</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="C21" s="32" t="s">
         <v>206</v>
-      </c>
-      <c r="C21" s="32" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="41" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" s="42" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C23" s="40">
         <v>42105</v>
@@ -2164,10 +2244,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B24" s="32" t="s">
         <v>212</v>
-      </c>
-      <c r="B24" s="32" t="s">
-        <v>213</v>
       </c>
       <c r="C24" s="40">
         <v>42328</v>
@@ -2175,7 +2255,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" s="32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C25" s="40">
         <v>42346</v>
@@ -2189,17 +2269,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A52"/>
+  <dimension ref="A1:A55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -2209,257 +2289,272 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>159</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>286</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>156</v>
+        <v>284</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>285</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>170</v>
+        <v>283</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>259</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>283</v>
+        <v>302</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>167</v>
+        <v>301</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>166</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>219</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>154</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>220</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>142</v>
+        <v>219</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>287</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="44" t="s">
-        <v>290</v>
+      <c r="A35" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>158</v>
+        <v>285</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>147</v>
+      <c r="A37" s="44" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>282</v>
+        <v>161</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>276</v>
+        <v>305</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>278</v>
+        <v>303</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>164</v>
+        <v>275</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>145</v>
+        <v>276</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>217</v>
+        <v>304</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>215</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>216</v>
+        <v>145</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>165</v>
+        <v>216</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>218</v>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:A52">
-    <sortCondition ref="A52"/>
+  <sortState ref="A1:A55">
+    <sortCondition ref="A55"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -2467,6 +2562,188 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>316</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B3" t="s">
+        <v>299</v>
+      </c>
+      <c r="D3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B4" t="s">
+        <v>299</v>
+      </c>
+      <c r="D4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>294</v>
+      </c>
+      <c r="D5" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>296</v>
+      </c>
+      <c r="D6" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>295</v>
+      </c>
+      <c r="D7" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>298</v>
+      </c>
+      <c r="B9" t="s">
+        <v>299</v>
+      </c>
+      <c r="D9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
@@ -2481,65 +2758,65 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="43" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B4" s="43" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4" s="43" t="s">
         <v>225</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="D4" s="43" t="s">
         <v>226</v>
-      </c>
-      <c r="D4" s="43" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="43" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B9" s="43" t="s">
+        <v>224</v>
+      </c>
+      <c r="C9" s="43" t="s">
         <v>225</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="D9" s="43" t="s">
         <v>226</v>
-      </c>
-      <c r="D9" s="43" t="s">
-        <v>227</v>
       </c>
       <c r="F9" s="43"/>
       <c r="G9" s="43"/>
@@ -2548,7 +2825,7 @@
     </row>
     <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G10" s="43"/>
       <c r="H10" s="43"/>
@@ -2556,77 +2833,77 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G17" s="43"/>
       <c r="H17" s="43"/>
@@ -2634,63 +2911,63 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G23" s="43"/>
       <c r="H23" s="43"/>
@@ -2698,49 +2975,49 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B24" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C24" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D24" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B25" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C25" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B26" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C26" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D26" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G28" s="43"/>
       <c r="H28" s="43"/>
@@ -2748,91 +3025,91 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B29" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C29" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D29" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B30" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C30" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D30" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D31" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B32" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C32" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D32" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B33" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C33" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D33" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B34" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C34" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G36" s="43"/>
       <c r="H36" s="43"/>
@@ -2840,49 +3117,49 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B37" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C37" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D37" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B38" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C38" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D38" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B39" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C39" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D39" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G41" s="43"/>
       <c r="H41" s="43"/>
@@ -2890,44 +3167,44 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B42" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C42" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D42" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B43" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C43" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D43" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B45" s="43" t="s">
+        <v>224</v>
+      </c>
+      <c r="C45" s="43" t="s">
         <v>225</v>
       </c>
-      <c r="C45" s="43" t="s">
+      <c r="D45" s="43" t="s">
         <v>226</v>
-      </c>
-      <c r="D45" s="43" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2950,7 +3227,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
@@ -3292,7 +3569,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A19"/>
   <sheetViews>
@@ -3304,92 +3581,92 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>